<commit_message>
trying to get tsp working without binary programming ... not going too well
</commit_message>
<xml_diff>
--- a/notebooks/simple-nlp/simple-nlp.xlsx
+++ b/notebooks/simple-nlp/simple-nlp.xlsx
@@ -8,25 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dbiagion/gitrepos/optimization-modeling-info-3440/notebooks/simple-nlp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4444B42A-6ED4-444E-84A9-9810DD52234C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63D358B-3644-5C49-BD06-91DA7C7DCD79}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33080" yWindow="-6480" windowWidth="27640" windowHeight="16540" xr2:uid="{342FC13A-667D-234F-B1C5-CF145304204A}"/>
+    <workbookView xWindow="-33080" yWindow="-6480" windowWidth="27640" windowHeight="16540" activeTab="1" xr2:uid="{342FC13A-667D-234F-B1C5-CF145304204A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ipopt" sheetId="1" r:id="rId1"/>
+    <sheet name="tsp" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$4:$B$204</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$4:$C$204</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$4:$B$204</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$4:$C$204</definedName>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$B$2</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">ipopt!$B$2</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$B$2</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$B$2</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">ipopt!$B$2</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">ipopt!$B$2</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
@@ -35,7 +32,7 @@
     <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$C$2</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">ipopt!$C$2</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
@@ -53,7 +50,7 @@
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -68,12 +65,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>y</t>
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
   </si>
 </sst>
 </file>
@@ -210,7 +225,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$204</c:f>
+              <c:f>ipopt!$B$4:$B$204</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="201"/>
@@ -822,7 +837,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$4:$C$204</c:f>
+              <c:f>ipopt!$C$4:$C$204</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="201"/>
@@ -2499,7 +2514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9030DE9-7B3F-774F-85CD-C7EAE57915D0}">
   <dimension ref="B1:C204"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -4338,4 +4353,183 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D2962F8-B287-5A41-8245-DDC42133CF2F}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <f>$M$3</f>
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>16</v>
+      </c>
+      <c r="D2">
+        <v>63</v>
+      </c>
+      <c r="E2">
+        <v>21</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="G2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>57</v>
+      </c>
+      <c r="C3">
+        <f>$M$3</f>
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>40</v>
+      </c>
+      <c r="E3">
+        <v>46</v>
+      </c>
+      <c r="F3">
+        <v>69</v>
+      </c>
+      <c r="G3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <f>$M$3</f>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>55</v>
+      </c>
+      <c r="F4">
+        <v>53</v>
+      </c>
+      <c r="G4">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>71</v>
+      </c>
+      <c r="C5">
+        <v>53</v>
+      </c>
+      <c r="D5">
+        <v>58</v>
+      </c>
+      <c r="E5">
+        <f>$M$3</f>
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>47</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>27</v>
+      </c>
+      <c r="C6">
+        <v>79</v>
+      </c>
+      <c r="D6">
+        <v>53</v>
+      </c>
+      <c r="E6">
+        <v>35</v>
+      </c>
+      <c r="F6">
+        <f>$M$3</f>
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>57</v>
+      </c>
+      <c r="C7">
+        <v>47</v>
+      </c>
+      <c r="D7">
+        <v>51</v>
+      </c>
+      <c r="E7">
+        <v>17</v>
+      </c>
+      <c r="F7">
+        <v>24</v>
+      </c>
+      <c r="G7">
+        <f>$M$3</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>